<commit_message>
Switch Rec 14b to 14a
</commit_message>
<xml_diff>
--- a/specification/Cards_OHSU_20221128_Control.xlsx
+++ b/specification/Cards_OHSU_20221128_Control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/shafferv_umsystem_edu/Documents/Other Grants/Dorr Koopman BP Proposals/COACH AHRQ U18 submission and revision/COACH Revision/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yateam/HTN/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{5818CCC2-1B61-D946-A545-AE76D11C13AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AB06FB1-D4E2-894B-AFD5-84DB6F12148B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8184565-0B07-5047-AF99-7749ED674981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="50940" windowHeight="26500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDSCards" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -472,12 +469,21 @@
     </comment>
     <comment ref="G20" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     difference between no BP goal non-harms and monitoring?
 Reply:
     will be same as monitoring no BP goal in the future</t>
+        </r>
       </text>
     </comment>
     <comment ref="E23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
@@ -584,7 +590,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="473">
   <si>
     <t>Recommendation #</t>
   </si>
@@ -739,9 +745,6 @@
   </si>
   <si>
     <t>Note that any reading in the last 2 weeks triggers this, so the note about checking again in 5 minutes may seem irrelevant in some cases.</t>
-  </si>
-  <si>
-    <t>HE-HypertensiveEmergencyIssued</t>
   </si>
   <si>
     <t>Alert: Blood pressure of &gt;180/120 mmHg recorded.</t>
@@ -2190,12 +2193,18 @@
   <si>
     <t>Use shared decision making for treatment. [Use the same phrase as above? Discuss using medication to treat high blood pressure with your care team.]</t>
   </si>
+  <si>
+    <t>HE-HypertensiveEmergencyEffective</t>
+  </si>
+  <si>
+    <t>14a and 14b were originally intended to separate patients who were "new" and only needed non-medicinal recommendations from those who had been working on goals for a period of time and should now be fed pharma recs too. Now, everyone receives both right away.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2244,13 +2253,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2393,7 +2395,25 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2408,25 +2428,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2730,10 +2732,10 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2807,11 +2809,11 @@
       <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
       <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
@@ -2892,11 +2894,11 @@
       <c r="E3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="23" t="s">
-        <v>439</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>443</v>
+      <c r="F3" s="16" t="s">
+        <v>438</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>442</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>37</v>
@@ -2940,10 +2942,10 @@
         <v>49</v>
       </c>
       <c r="W3" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="X3" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:24" s="5" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -2951,50 +2953,50 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="23" t="s">
-        <v>444</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>40</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6" t="s">
@@ -3003,10 +3005,10 @@
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="W4" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="X4" s="6"/>
     </row>
@@ -3015,31 +3017,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="17" t="s">
+        <v>439</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="24" t="s">
-        <v>440</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>448</v>
-      </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>40</v>
@@ -3049,34 +3051,34 @@
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>43</v>
       </c>
       <c r="P5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="R5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="U5" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="W5" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="X5" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -3084,31 +3086,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="17" t="s">
+        <v>439</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>444</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="24" t="s">
-        <v>440</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>445</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>40</v>
@@ -3118,32 +3120,32 @@
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>43</v>
       </c>
       <c r="P6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q6" s="15" t="s">
         <v>73</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>74</v>
       </c>
       <c r="R6" s="6"/>
       <c r="S6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="T6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="U6" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="W6" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="W6" s="5" t="s">
+      <c r="X6" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -3151,31 +3153,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="17" t="s">
+        <v>440</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>445</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="24" t="s">
-        <v>441</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>446</v>
-      </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>40</v>
@@ -3185,32 +3187,32 @@
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>43</v>
       </c>
       <c r="P7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q7" s="15" t="s">
         <v>73</v>
-      </c>
-      <c r="Q7" s="15" t="s">
-        <v>74</v>
       </c>
       <c r="R7" s="6"/>
       <c r="S7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="T7" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="U7" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="W7" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="W7" s="5" t="s">
+      <c r="X7" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:24" s="5" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -3218,31 +3220,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="17" t="s">
+        <v>441</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="24" t="s">
-        <v>442</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>447</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>40</v>
@@ -3252,27 +3254,27 @@
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="P8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q8" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="U8" s="6"/>
       <c r="W8" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X8" s="6"/>
     </row>
@@ -3281,66 +3283,66 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>40</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>43</v>
       </c>
       <c r="P9" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q9" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>117</v>
       </c>
       <c r="R9" s="8"/>
       <c r="S9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="T9" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="U9" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="U9" s="8" t="s">
+      <c r="W9" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="W9" s="7" t="s">
+      <c r="X9" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="X9" s="8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:24" s="7" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
@@ -3349,42 +3351,42 @@
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="I10" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>40</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
       <c r="S10" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
@@ -3396,44 +3398,44 @@
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="I11" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>134</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>40</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R11" s="8"/>
       <c r="S11" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
@@ -3445,44 +3447,44 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="I12" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="J12" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>40</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M12" s="8"/>
       <c r="N12" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R12" s="8"/>
       <c r="S12" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
@@ -3490,27 +3492,27 @@
     </row>
     <row r="13" spans="1:24" s="7" customFormat="1" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>148</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
@@ -3519,7 +3521,7 @@
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
@@ -3532,50 +3534,50 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="I14" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="J14" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="K14" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="L14" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="M14" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="N14" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>161</v>
       </c>
       <c r="O14" s="8"/>
       <c r="P14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q14" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="R14" s="8"/>
       <c r="S14" s="8" t="s">
@@ -3584,10 +3586,10 @@
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
       <c r="V14" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="W14" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="W14" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="X14" s="8"/>
     </row>
@@ -3596,53 +3598,53 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>449</v>
-      </c>
-      <c r="H15" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>167</v>
-      </c>
       <c r="J15" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>40</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="O15" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="P15" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q15" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="Q15" s="6" t="s">
-        <v>169</v>
-      </c>
       <c r="R15" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S15" s="6" t="s">
         <v>15</v>
@@ -3650,37 +3652,37 @@
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
       <c r="W15" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X15" s="6"/>
     </row>
     <row r="16" spans="1:24" s="5" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="G16" s="16" t="s">
+        <v>449</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="G16" s="23" t="s">
-        <v>450</v>
-      </c>
-      <c r="H16" s="5" t="s">
+      <c r="I16" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>176</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>40</v>
@@ -3690,102 +3692,102 @@
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O16" s="6" t="s">
         <v>43</v>
       </c>
       <c r="P16" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q16" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="Q16" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="R16" s="6"/>
       <c r="S16" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T16" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="U16" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="U16" s="6" t="s">
+      <c r="V16" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="V16" s="5" t="s">
+      <c r="W16" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="W16" s="5" t="s">
+      <c r="X16" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="X16" s="6" t="s">
+    </row>
+    <row r="17" spans="1:24" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="T17" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>451</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q17" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="T17" s="6" t="s">
+      <c r="U17" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="U17" s="6" t="s">
+      <c r="V17" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="W17" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="V17" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="W17" s="5" t="s">
+      <c r="X17" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="X17" s="6" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:24" s="7" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
@@ -3793,63 +3795,63 @@
         <v>15</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>193</v>
-      </c>
       <c r="H18" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>40</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M18" s="8"/>
       <c r="N18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O18" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O18" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="P18" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q18" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="Q18" s="8" t="s">
-        <v>169</v>
-      </c>
       <c r="R18" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S18" s="8" t="s">
         <v>15</v>
       </c>
       <c r="T18" s="8"/>
       <c r="U18" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="V18" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="V18" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="X18" s="8"/>
     </row>
@@ -3858,66 +3860,66 @@
         <v>16</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="I19" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>199</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>40</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M19" s="8"/>
       <c r="N19" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O19" s="8" t="s">
         <v>43</v>
       </c>
       <c r="P19" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q19" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="Q19" s="8" t="s">
-        <v>117</v>
       </c>
       <c r="R19" s="8"/>
       <c r="S19" s="8" t="s">
         <v>15</v>
       </c>
       <c r="T19" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U19" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="W19" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="W19" s="7" t="s">
-        <v>201</v>
-      </c>
       <c r="X19" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:24" s="7" customFormat="1" ht="96" hidden="1" x14ac:dyDescent="0.2">
@@ -3925,54 +3927,54 @@
         <v>17</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="E20" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="G20" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="H20" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I20" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="I20" s="7" t="s">
+      <c r="J20" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="K20" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="L20" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="N20" s="8" t="s">
         <v>210</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="N20" s="8" t="s">
-        <v>211</v>
       </c>
       <c r="O20" s="8"/>
       <c r="P20" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q20" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R20" s="8"/>
       <c r="S20" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
@@ -3980,90 +3982,90 @@
     </row>
     <row r="21" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>451</v>
+      </c>
+      <c r="K21" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="F21" s="24" t="s">
-        <v>225</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>452</v>
-      </c>
-      <c r="K21" s="6" t="s">
+      <c r="L21" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="M21" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q21" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="Q21" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="R21" s="6"/>
       <c r="S21" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
       <c r="W21" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X21" s="6"/>
     </row>
     <row r="22" spans="1:24" s="5" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="G22" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="K22" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L22" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>227</v>
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q22" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="Q22" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="R22" s="6"/>
       <c r="S22" s="6" t="s">
@@ -4072,101 +4074,101 @@
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
       <c r="V22" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="W22" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X22" s="6"/>
     </row>
     <row r="23" spans="1:24" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C23" s="21" t="s">
+      <c r="D23" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="D23" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="E23" s="21" t="s">
+      <c r="F23" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="G23" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="H23" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="I23" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="I23" s="21" t="s">
+      <c r="J23" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="J23" s="21" t="s">
+      <c r="K23" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="L23" s="6" t="s">
         <v>237</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>238</v>
       </c>
       <c r="M23" s="6"/>
       <c r="N23" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="O23" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="O23" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="P23" s="16" t="s">
+      <c r="P23" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q23" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="Q23" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="R23" s="16"/>
+      <c r="R23" s="18"/>
       <c r="S23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
       <c r="W23" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="X23" s="6"/>
     </row>
     <row r="24" spans="1:24" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
       <c r="K24" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L24" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="M24" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="N24" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="N24" s="6" t="s">
-        <v>244</v>
-      </c>
       <c r="O24" s="6"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
       <c r="S24" s="6" t="s">
         <v>15</v>
       </c>
@@ -4176,50 +4178,50 @@
     </row>
     <row r="25" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="H25" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="H25" s="5" t="s">
-        <v>250</v>
-      </c>
       <c r="J25" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L25" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="M25" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="M25" s="6" t="s">
+      <c r="N25" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>244</v>
       </c>
       <c r="O25" s="6"/>
       <c r="P25" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q25" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="Q25" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="R25" s="6"/>
       <c r="S25" s="6" t="s">
@@ -4228,96 +4230,96 @@
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
       <c r="W25" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="X25" s="6"/>
     </row>
     <row r="26" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>453</v>
+      <c r="F26" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>452</v>
       </c>
       <c r="K26" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L26" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="M26" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q26" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="Q26" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="R26" s="6"/>
       <c r="S26" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T26" s="6"/>
       <c r="U26" s="6"/>
       <c r="W26" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X26" s="6"/>
     </row>
     <row r="27" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="G27" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="G27" s="23" t="s">
-        <v>261</v>
-      </c>
       <c r="K27" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q27" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="Q27" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="R27" s="6"/>
       <c r="S27" s="6" t="s">
@@ -4326,62 +4328,62 @@
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
       <c r="W27" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X27" s="6"/>
     </row>
     <row r="28" spans="1:24" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="C28" s="21" t="s">
+      <c r="D28" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="D28" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="E28" s="21" t="s">
+      <c r="F28" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="G28" s="20" t="s">
+        <v>453</v>
+      </c>
+      <c r="H28" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="G28" s="25" t="s">
-        <v>454</v>
-      </c>
-      <c r="H28" s="21" t="s">
+      <c r="I28" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="J28" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="I28" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="J28" s="21" t="s">
+      <c r="K28" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="L28" s="6" t="s">
         <v>267</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>268</v>
       </c>
       <c r="M28" s="6"/>
       <c r="N28" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="O28" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="O28" s="6" t="s">
+      <c r="P28" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q28" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="P28" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q28" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="R28" s="16" t="s">
-        <v>75</v>
+      <c r="R28" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="S28" s="6" t="s">
         <v>15</v>
@@ -4389,96 +4391,96 @@
       <c r="T28" s="6"/>
       <c r="U28" s="6"/>
       <c r="W28" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="X28" s="6"/>
     </row>
     <row r="29" spans="1:24" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
       <c r="K29" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L29" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="M29" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="M29" s="6" t="s">
+      <c r="N29" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="N29" s="6" t="s">
-        <v>275</v>
-      </c>
       <c r="O29" s="6"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
       <c r="S29" s="6" t="s">
         <v>15</v>
       </c>
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
       <c r="W29" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="X29" s="6"/>
     </row>
     <row r="30" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="G30" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="H30" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="G30" s="23" t="s">
-        <v>455</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>281</v>
-      </c>
       <c r="I30" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L30" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="M30" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="M30" s="6" t="s">
+      <c r="N30" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="O30" s="6"/>
       <c r="P30" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q30" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="Q30" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="R30" s="6"/>
       <c r="S30" s="6" t="s">
@@ -4490,90 +4492,90 @@
     </row>
     <row r="31" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="D31" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="G31" s="24" t="s">
-        <v>456</v>
+      <c r="G31" s="17" t="s">
+        <v>455</v>
       </c>
       <c r="K31" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L31" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L31" s="6" t="s">
+      <c r="M31" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q31" s="6" t="s">
         <v>286</v>
-      </c>
-      <c r="Q31" s="6" t="s">
-        <v>287</v>
       </c>
       <c r="R31" s="6"/>
       <c r="S31" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T31" s="6"/>
       <c r="U31" s="6"/>
       <c r="W31" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X31" s="6"/>
     </row>
     <row r="32" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="D32" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="F32" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="F32" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="G32" s="24" t="s">
-        <v>457</v>
+      <c r="G32" s="17" t="s">
+        <v>456</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
       <c r="P32" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q32" s="6" t="s">
         <v>286</v>
-      </c>
-      <c r="Q32" s="6" t="s">
-        <v>287</v>
       </c>
       <c r="R32" s="6"/>
       <c r="S32" s="6" t="s">
@@ -4582,61 +4584,61 @@
       <c r="T32" s="6"/>
       <c r="U32" s="6"/>
       <c r="W32" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X32" s="6"/>
     </row>
     <row r="33" spans="1:24" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C33" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="C33" s="21" t="s">
+      <c r="D33" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="E33" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="D33" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="E33" s="21" t="s">
+      <c r="F33" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="G33" s="20" t="s">
+        <v>457</v>
+      </c>
+      <c r="H33" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="G33" s="25" t="s">
-        <v>458</v>
-      </c>
-      <c r="H33" s="21" t="s">
+      <c r="I33" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="J33" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="I33" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="J33" s="21" t="s">
+      <c r="K33" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="L33" s="6" t="s">
         <v>297</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>298</v>
       </c>
       <c r="M33" s="6"/>
       <c r="N33" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="O33" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="O33" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="P33" s="16" t="s">
+      <c r="P33" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q33" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="Q33" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="R33" s="16"/>
+      <c r="R33" s="18"/>
       <c r="S33" s="6" t="s">
         <v>15</v>
       </c>
@@ -4645,82 +4647,82 @@
       <c r="X33" s="6"/>
     </row>
     <row r="34" spans="1:24" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
       <c r="K34" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L34" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="M34" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="M34" s="6" t="s">
+      <c r="N34" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="N34" s="6" t="s">
-        <v>303</v>
-      </c>
       <c r="O34" s="6"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
       <c r="S34" s="6" t="s">
         <v>15</v>
       </c>
       <c r="T34" s="6"/>
       <c r="U34" s="6"/>
       <c r="W34" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="X34" s="6"/>
     </row>
     <row r="35" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="D35" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="17" t="s">
+        <v>458</v>
+      </c>
+      <c r="G35" s="16" t="s">
         <v>459</v>
       </c>
-      <c r="G35" s="23" t="s">
-        <v>460</v>
-      </c>
       <c r="K35" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L35" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="M35" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="M35" s="6" t="s">
+      <c r="N35" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="N35" s="6" t="s">
-        <v>303</v>
       </c>
       <c r="O35" s="6"/>
       <c r="P35" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q35" s="6" t="s">
         <v>286</v>
-      </c>
-      <c r="Q35" s="6" t="s">
-        <v>287</v>
       </c>
       <c r="R35" s="6"/>
       <c r="S35" s="6" t="s">
@@ -4729,52 +4731,52 @@
       <c r="T35" s="6"/>
       <c r="U35" s="6"/>
       <c r="V35" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="W35" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="W35" s="5" t="s">
-        <v>309</v>
       </c>
       <c r="X35" s="6"/>
     </row>
     <row r="36" spans="1:24" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>311</v>
-      </c>
       <c r="D36" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>316</v>
-      </c>
-      <c r="G36" s="24" t="s">
-        <v>461</v>
+        <v>203</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>460</v>
       </c>
       <c r="K36" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L36" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L36" s="6" t="s">
+      <c r="M36" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="M36" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q36" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="Q36" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="R36" s="6"/>
       <c r="S36" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T36" s="6"/>
       <c r="U36" s="6"/>
@@ -4782,22 +4784,22 @@
     </row>
     <row r="37" spans="1:24" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F37" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F37" s="23" t="s">
+      <c r="G37" s="16" t="s">
         <v>316</v>
-      </c>
-      <c r="G37" s="23" t="s">
-        <v>317</v>
       </c>
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
@@ -4805,10 +4807,10 @@
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q37" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="Q37" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="R37" s="6"/>
       <c r="S37" s="6" t="s">
@@ -4817,143 +4819,143 @@
       <c r="T37" s="6"/>
       <c r="U37" s="6"/>
       <c r="W37" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X37" s="6"/>
     </row>
     <row r="38" spans="1:24" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C38" s="19" t="s">
         <v>318</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="C38" s="21" t="s">
+      <c r="D38" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="20" t="s">
+        <v>462</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="H38" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="D38" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="E38" s="21"/>
-      <c r="F38" s="25" t="s">
-        <v>463</v>
-      </c>
-      <c r="G38" s="25" t="s">
-        <v>464</v>
-      </c>
-      <c r="H38" s="21" t="s">
+      <c r="I38" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="J38" s="19" t="s">
         <v>320</v>
       </c>
-      <c r="I38" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="J38" s="21" t="s">
+      <c r="K38" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="L38" s="6" t="s">
         <v>321</v>
-      </c>
-      <c r="K38" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="L38" s="6" t="s">
-        <v>322</v>
       </c>
       <c r="M38" s="6"/>
       <c r="N38" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="O38" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="O38" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="P38" s="16" t="s">
+      <c r="P38" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q38" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="Q38" s="16" t="s">
-        <v>313</v>
-      </c>
-      <c r="R38" s="16"/>
+      <c r="R38" s="18"/>
       <c r="S38" s="6" t="s">
         <v>15</v>
       </c>
       <c r="T38" s="6"/>
       <c r="U38" s="6"/>
       <c r="W38" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X38" s="6"/>
     </row>
     <row r="39" spans="1:24" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
       <c r="K39" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L39" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="M39" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="M39" s="6" t="s">
+      <c r="N39" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="N39" s="6" t="s">
-        <v>327</v>
-      </c>
       <c r="O39" s="6"/>
-      <c r="P39" s="16"/>
-      <c r="Q39" s="16"/>
-      <c r="R39" s="16"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
       <c r="S39" s="6" t="s">
         <v>15</v>
       </c>
       <c r="T39" s="6"/>
       <c r="U39" s="6"/>
       <c r="W39" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="X39" s="6"/>
     </row>
     <row r="40" spans="1:24" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F40" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="G40" s="23" t="s">
-        <v>466</v>
+      <c r="G40" s="16" t="s">
+        <v>465</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L40" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="M40" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="M40" s="6" t="s">
+      <c r="N40" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="N40" s="6" t="s">
-        <v>327</v>
       </c>
       <c r="O40" s="6"/>
       <c r="P40" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q40" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="Q40" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="R40" s="6"/>
       <c r="S40" s="6" t="s">
@@ -4962,52 +4964,52 @@
       <c r="T40" s="6"/>
       <c r="U40" s="6"/>
       <c r="V40" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="W40" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="X40" s="6"/>
     </row>
     <row r="41" spans="1:24" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="D41" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="G41" s="24" t="s">
-        <v>462</v>
+      <c r="G41" s="17" t="s">
+        <v>461</v>
       </c>
       <c r="K41" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="L41" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L41" s="6" t="s">
+      <c r="M41" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
       <c r="P41" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q41" s="6" t="s">
         <v>336</v>
-      </c>
-      <c r="Q41" s="6" t="s">
-        <v>337</v>
       </c>
       <c r="R41" s="6"/>
       <c r="S41" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
@@ -5015,22 +5017,22 @@
     </row>
     <row r="42" spans="1:24" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C42" s="5" t="s">
+      <c r="D42" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F42" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F42" s="23" t="s">
+      <c r="G42" s="16" t="s">
         <v>340</v>
-      </c>
-      <c r="G42" s="23" t="s">
-        <v>341</v>
       </c>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
@@ -5038,10 +5040,10 @@
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
       <c r="P42" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q42" s="6" t="s">
         <v>336</v>
-      </c>
-      <c r="Q42" s="6" t="s">
-        <v>337</v>
       </c>
       <c r="R42" s="6"/>
       <c r="S42" s="6" t="s">
@@ -5052,52 +5054,52 @@
       <c r="X42" s="6"/>
     </row>
     <row r="43" spans="1:24" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C43" s="19" t="s">
         <v>342</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="C43" s="21" t="s">
+      <c r="D43" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="E43" s="19"/>
+      <c r="F43" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="D43" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="E43" s="21"/>
-      <c r="F43" s="16" t="s">
+      <c r="G43" s="22" t="s">
+        <v>464</v>
+      </c>
+      <c r="H43" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="G43" s="26" t="s">
-        <v>465</v>
-      </c>
-      <c r="H43" s="21" t="s">
+      <c r="I43" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="J43" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="I43" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="J43" s="21" t="s">
+      <c r="K43" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="L43" s="6" t="s">
         <v>346</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>347</v>
       </c>
       <c r="M43" s="6"/>
       <c r="N43" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="O43" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="O43" s="6" t="s">
-        <v>349</v>
-      </c>
       <c r="P43" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q43" s="6" t="s">
         <v>336</v>
-      </c>
-      <c r="Q43" s="6" t="s">
-        <v>337</v>
       </c>
       <c r="R43" s="6"/>
       <c r="S43" s="6" t="s">
@@ -5108,34 +5110,34 @@
       <c r="X43" s="6"/>
     </row>
     <row r="44" spans="1:24" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
       <c r="K44" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L44" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="M44" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="M44" s="6" t="s">
+      <c r="N44" s="6" t="s">
         <v>351</v>
-      </c>
-      <c r="N44" s="6" t="s">
-        <v>352</v>
       </c>
       <c r="O44" s="6"/>
       <c r="P44" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q44" s="6" t="s">
         <v>336</v>
-      </c>
-      <c r="Q44" s="6" t="s">
-        <v>337</v>
       </c>
       <c r="R44" s="6"/>
       <c r="S44" s="6" t="s">
@@ -5144,47 +5146,47 @@
       <c r="T44" s="6"/>
       <c r="U44" s="6"/>
       <c r="W44" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="X44" s="6"/>
     </row>
     <row r="45" spans="1:24" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="D45" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F45" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="G45" s="24" t="s">
-        <v>467</v>
+      <c r="G45" s="17" t="s">
+        <v>466</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L45" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="M45" s="6" t="s">
+      <c r="N45" s="6" t="s">
         <v>351</v>
-      </c>
-      <c r="N45" s="6" t="s">
-        <v>352</v>
       </c>
       <c r="O45" s="6"/>
       <c r="P45" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q45" s="6" t="s">
         <v>336</v>
-      </c>
-      <c r="Q45" s="6" t="s">
-        <v>337</v>
       </c>
       <c r="R45" s="6"/>
       <c r="S45" s="6" t="s">
@@ -5193,10 +5195,10 @@
       <c r="T45" s="6"/>
       <c r="U45" s="6"/>
       <c r="V45" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="W45" s="5" t="s">
         <v>357</v>
-      </c>
-      <c r="W45" s="5" t="s">
-        <v>358</v>
       </c>
       <c r="X45" s="6"/>
     </row>
@@ -5206,20 +5208,20 @@
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="D46" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="F46" s="8" t="s">
         <v>360</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>361</v>
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="I46" s="7" t="s">
         <v>362</v>
-      </c>
-      <c r="I46" s="7" t="s">
-        <v>363</v>
       </c>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
@@ -5240,20 +5242,20 @@
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="F47" s="8" t="s">
         <v>364</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>365</v>
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="I47" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="I47" s="7" t="s">
+      <c r="J47" s="7" t="s">
         <v>367</v>
-      </c>
-      <c r="J47" s="7" t="s">
-        <v>368</v>
       </c>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
@@ -5274,17 +5276,17 @@
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="F48" s="8" t="s">
         <v>369</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>370</v>
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
@@ -5305,17 +5307,17 @@
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
@@ -5336,20 +5338,20 @@
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="F50" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>375</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="I50" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="I50" s="7" t="s">
+      <c r="J50" s="7" t="s">
         <v>377</v>
-      </c>
-      <c r="J50" s="7" t="s">
-        <v>378</v>
       </c>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
@@ -5357,13 +5359,13 @@
       <c r="N50" s="8"/>
       <c r="O50" s="8"/>
       <c r="P50" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q50" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="Q50" s="8" t="s">
-        <v>380</v>
-      </c>
       <c r="R50" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S50" s="8"/>
       <c r="T50" s="8"/>
@@ -5376,20 +5378,20 @@
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G51" s="8"/>
       <c r="H51" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="J51" s="7" t="s">
         <v>382</v>
-      </c>
-      <c r="I51" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="J51" s="7" t="s">
-        <v>383</v>
       </c>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
@@ -5397,13 +5399,13 @@
       <c r="N51" s="8"/>
       <c r="O51" s="8"/>
       <c r="P51" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q51" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="Q51" s="8" t="s">
-        <v>380</v>
-      </c>
       <c r="R51" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="S51" s="8"/>
       <c r="T51" s="8"/>
@@ -5415,35 +5417,35 @@
         <v>29</v>
       </c>
       <c r="B52" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="F52" s="17" t="s">
+        <v>467</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>468</v>
+      </c>
+      <c r="H52" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="F52" s="24" t="s">
-        <v>468</v>
-      </c>
-      <c r="G52" s="27" t="s">
-        <v>469</v>
-      </c>
-      <c r="H52" s="5" t="s">
+      <c r="I52" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="J52" s="5" t="s">
         <v>387</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>388</v>
       </c>
       <c r="K52" s="6" t="s">
         <v>40</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M52" s="6"/>
       <c r="N52" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O52" s="6" t="s">
         <v>43</v>
@@ -5452,19 +5454,19 @@
       <c r="Q52" s="6"/>
       <c r="R52" s="6"/>
       <c r="S52" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T52" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="U52" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="U52" s="6" t="s">
+      <c r="W52" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="W52" s="5" t="s">
+      <c r="X52" s="6" t="s">
         <v>392</v>
-      </c>
-      <c r="X52" s="6" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="53" spans="1:24" s="7" customFormat="1" ht="64" hidden="1" x14ac:dyDescent="0.2">
@@ -5473,19 +5475,19 @@
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="F53" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="G53" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="H53" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="H53" s="7" t="s">
+      <c r="I53" s="7" t="s">
         <v>397</v>
-      </c>
-      <c r="I53" s="7" t="s">
-        <v>398</v>
       </c>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
@@ -5506,32 +5508,32 @@
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="G54" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="H54" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="H54" s="7" t="s">
+      <c r="I54" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="I54" s="7" t="s">
+      <c r="J54" s="7" t="s">
         <v>403</v>
-      </c>
-      <c r="J54" s="7" t="s">
-        <v>404</v>
       </c>
       <c r="K54" s="8" t="s">
         <v>40</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M54" s="8"/>
       <c r="N54" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O54" s="8" t="s">
         <v>43</v>
@@ -5543,7 +5545,7 @@
       <c r="T54" s="8"/>
       <c r="U54" s="8"/>
       <c r="V54" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="X54" s="8"/>
     </row>
@@ -5552,35 +5554,35 @@
         <v>32</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C55" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="F55" s="16" t="s">
+        <v>470</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>469</v>
+      </c>
+      <c r="H55" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="F55" s="23" t="s">
-        <v>471</v>
-      </c>
-      <c r="G55" s="24" t="s">
-        <v>470</v>
-      </c>
-      <c r="H55" s="5" t="s">
+      <c r="I55" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="J55" s="5" t="s">
         <v>407</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>408</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>40</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M55" s="6"/>
       <c r="N55" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O55" s="6" t="s">
         <v>43</v>
@@ -5589,19 +5591,19 @@
       <c r="Q55" s="6"/>
       <c r="R55" s="6"/>
       <c r="S55" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T55" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="U55" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="U55" s="6" t="s">
+      <c r="W55" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="W55" s="5" t="s">
+      <c r="X55" s="6" t="s">
         <v>411</v>
-      </c>
-      <c r="X55" s="6" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="56" spans="1:24" s="5" customFormat="1" ht="64" x14ac:dyDescent="0.2">
@@ -5609,32 +5611,32 @@
         <v>33</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="F56" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="F56" s="23" t="s">
+      <c r="G56" s="16" t="s">
         <v>415</v>
       </c>
-      <c r="G56" s="23" t="s">
+      <c r="H56" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="H56" s="5" t="s">
-        <v>417</v>
-      </c>
       <c r="I56" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K56" s="6" t="s">
         <v>40</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M56" s="6"/>
       <c r="N56" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="O56" s="6" t="s">
         <v>43</v>
@@ -5646,16 +5648,16 @@
         <v>46</v>
       </c>
       <c r="T56" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="U56" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="U56" s="6" t="s">
+      <c r="W56" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="W56" s="5" t="s">
+      <c r="X56" s="6" t="s">
         <v>422</v>
-      </c>
-      <c r="X56" s="6" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="57" spans="1:24" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -5663,29 +5665,29 @@
         <v>34</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C57" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="F57" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="F57" s="23" t="s">
+      <c r="G57" s="16" t="s">
         <v>425</v>
       </c>
-      <c r="G57" s="23" t="s">
+      <c r="H57" s="5" t="s">
         <v>426</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>427</v>
       </c>
       <c r="K57" s="6" t="s">
         <v>40</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M57" s="6"/>
       <c r="N57" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O57" s="6" t="s">
         <v>43</v>
@@ -5694,19 +5696,19 @@
       <c r="Q57" s="6"/>
       <c r="R57" s="6"/>
       <c r="S57" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T57" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="U57" s="6" t="s">
         <v>428</v>
       </c>
-      <c r="U57" s="6" t="s">
+      <c r="W57" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="X57" s="6" t="s">
         <v>429</v>
-      </c>
-      <c r="W57" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="X57" s="6" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="58" spans="1:24" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -5715,10 +5717,10 @@
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="F58" s="10" t="s">
         <v>431</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>432</v>
       </c>
       <c r="G58" s="10"/>
       <c r="K58" s="10"/>
@@ -5740,10 +5742,10 @@
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="F59" s="10" t="s">
         <v>433</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>434</v>
       </c>
       <c r="G59" s="10"/>
       <c r="K59" s="10"/>
@@ -5765,10 +5767,10 @@
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="F60" s="10" t="s">
         <v>435</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>436</v>
       </c>
       <c r="G60" s="10"/>
       <c r="K60" s="10"/>
@@ -5790,10 +5792,10 @@
       </c>
       <c r="B61" s="10"/>
       <c r="C61" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="F61" s="10" t="s">
         <v>437</v>
-      </c>
-      <c r="F61" s="10" t="s">
-        <v>438</v>
       </c>
       <c r="G61" s="10"/>
       <c r="K61" s="10"/>
@@ -5812,6 +5814,53 @@
   </sheetData>
   <autoFilter ref="A4:X4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="63">
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="R23:R24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="R28:R29"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="Q33:Q34"/>
+    <mergeCell ref="R33:R34"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="P28:P29"/>
     <mergeCell ref="Q38:Q39"/>
     <mergeCell ref="R38:R39"/>
     <mergeCell ref="A43:A44"/>
@@ -5828,53 +5877,6 @@
     <mergeCell ref="J38:J39"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="C38:C39"/>
-    <mergeCell ref="R28:R29"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="Q33:Q34"/>
-    <mergeCell ref="R33:R34"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="Q28:Q29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="R23:R24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -5909,15 +5911,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003BCBFB114661454793731818D5E6868B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="438c95de508b09f83c8cd22ebab684c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5667dfd7-f4e3-48cd-9014-0118885df145" xmlns:ns4="b1b30e76-7c8b-48d4-a609-e5264444a5d4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5a43e309cb4e1e38cdb59c6ab3c5cfb6" ns3:_="" ns4:_="">
     <xsd:import namespace="5667dfd7-f4e3-48cd-9014-0118885df145"/>
@@ -6146,6 +6139,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6155,14 +6157,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4F029C2-E970-4B07-932F-A1CCEA214868}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20B0575C-424C-42DE-9583-4B052FD746DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6177,6 +6171,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4F029C2-E970-4B07-932F-A1CCEA214868}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>